<commit_message>
second commit updated name's and count
</commit_message>
<xml_diff>
--- a/resorces/API_DocsService_Automation.xlsx
+++ b/resorces/API_DocsService_Automation.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NG2574\API_workspace\AutomationTest\resorces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1324382E-44B4-4325-9994-246A579E6E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94764168-4084-4897-9BA7-9FD46F92635E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9BA805C0-0875-4538-96C9-7DEF9D6D0682}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="109">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -61,9 +61,6 @@
     <t>200</t>
   </si>
   <si>
-    <t>73</t>
-  </si>
-  <si>
     <t>Upload_doc_Body</t>
   </si>
   <si>
@@ -359,12 +356,19 @@
   </si>
   <si>
     <t>Successfully uploaded file to S3</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>Signed Agreement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -742,30 +746,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A271B4A6-3650-427D-A3F2-C5C9219B2B2E}">
-  <dimension ref="A1:BY18"/>
+  <dimension ref="A1:BZ18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
-    <col min="2" max="3" width="17.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="28.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="21.140625" collapsed="true"/>
+    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -774,23 +778,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
@@ -805,334 +809,337 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" t="s">
+        <v>40</v>
+      </c>
+      <c r="W5" t="s">
+        <v>41</v>
+      </c>
+      <c r="X5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>74</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>75</v>
+      </c>
+      <c r="BF5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BL5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>83</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>84</v>
+      </c>
+      <c r="BO5" t="s">
+        <v>85</v>
+      </c>
+      <c r="BP5" t="s">
+        <v>86</v>
+      </c>
+      <c r="BQ5" t="s">
+        <v>87</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>88</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>89</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>90</v>
+      </c>
+      <c r="BU5" t="s">
+        <v>91</v>
+      </c>
+      <c r="BV5" t="s">
+        <v>92</v>
+      </c>
+      <c r="BW5" t="s">
+        <v>93</v>
+      </c>
+      <c r="BX5" t="s">
+        <v>94</v>
+      </c>
+      <c r="BY5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>36</v>
-      </c>
-      <c r="R5" t="s">
-        <v>37</v>
-      </c>
-      <c r="S5" t="s">
-        <v>38</v>
-      </c>
-      <c r="T5" t="s">
-        <v>39</v>
-      </c>
-      <c r="U5" t="s">
-        <v>40</v>
-      </c>
-      <c r="V5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W5" t="s">
-        <v>42</v>
-      </c>
-      <c r="X5" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>61</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>72</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>73</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>74</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>75</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>76</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>77</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>78</v>
-      </c>
-      <c r="BH5" t="s">
-        <v>79</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>80</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>81</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>82</v>
-      </c>
-      <c r="BL5" t="s">
-        <v>83</v>
-      </c>
-      <c r="BM5" t="s">
-        <v>84</v>
-      </c>
-      <c r="BN5" t="s">
-        <v>85</v>
-      </c>
-      <c r="BO5" t="s">
-        <v>86</v>
-      </c>
-      <c r="BP5" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ5" t="s">
-        <v>88</v>
-      </c>
-      <c r="BR5" t="s">
-        <v>89</v>
-      </c>
-      <c r="BS5" t="s">
-        <v>90</v>
-      </c>
-      <c r="BT5" t="s">
-        <v>91</v>
-      </c>
-      <c r="BU5" t="s">
-        <v>92</v>
-      </c>
-      <c r="BV5" t="s">
-        <v>93</v>
-      </c>
-      <c r="BW5" t="s">
-        <v>94</v>
-      </c>
-      <c r="BX5" t="s">
+      <c r="BZ5" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
         <v>95</v>
       </c>
-      <c r="BY5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="D6" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" x14ac:dyDescent="0.25">
       <c r="D12" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s">
         <v>105</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="13" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="E15" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
-      <c r="E16" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>